<commit_message>
Added:expiry_automate_with_master, user_table, db_transfer_file, Updated:excel_table
</commit_message>
<xml_diff>
--- a/symbols.xlsx
+++ b/symbols.xlsx
@@ -496,7 +496,7 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>45434</v>
+        <v>45441</v>
       </c>
     </row>
     <row r="7">
@@ -506,7 +506,7 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>45441</v>
+        <v>45448</v>
       </c>
     </row>
     <row r="8">
@@ -516,7 +516,7 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>45433</v>
+        <v>45440</v>
       </c>
     </row>
     <row r="9">
@@ -526,7 +526,7 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>45440</v>
+        <v>45447</v>
       </c>
     </row>
     <row r="10">

</xml_diff>

<commit_message>
different data displayed upon refresh error fixed, x-axis 0 not displayed
</commit_message>
<xml_diff>
--- a/symbols.xlsx
+++ b/symbols.xlsx
@@ -496,7 +496,7 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>45489</v>
+        <v>45497</v>
       </c>
     </row>
     <row r="7">
@@ -506,7 +506,7 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>45497</v>
+        <v>45504</v>
       </c>
     </row>
     <row r="8">
@@ -516,7 +516,7 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>45489</v>
+        <v>45496</v>
       </c>
     </row>
     <row r="9">
@@ -526,7 +526,7 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>45496</v>
+        <v>45503</v>
       </c>
     </row>
     <row r="10">

</xml_diff>

<commit_message>
modified stop_iv_chart(killing cmdline), added interpolating of iv data(mean of missing iv data for greater and lesser strike, table calculated after 9:15(changed query)
</commit_message>
<xml_diff>
--- a/symbols.xlsx
+++ b/symbols.xlsx
@@ -456,7 +456,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>45491</v>
+        <v>45498</v>
       </c>
     </row>
     <row r="3">
@@ -466,7 +466,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
     </row>
     <row r="4">
@@ -516,7 +516,7 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>45496</v>
+        <v>45503</v>
       </c>
     </row>
     <row r="9">
@@ -526,7 +526,7 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>45503</v>
+        <v>45510</v>
       </c>
     </row>
     <row r="10">
@@ -536,7 +536,7 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>45495</v>
+        <v>45502</v>
       </c>
     </row>
     <row r="11">
@@ -546,7 +546,7 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>45502</v>
+        <v>45509</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified stop_iv_chart, progress bar added in update_master
</commit_message>
<xml_diff>
--- a/symbols.xlsx
+++ b/symbols.xlsx
@@ -456,7 +456,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
     </row>
     <row r="3">
@@ -466,7 +466,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>45505</v>
+        <v>45512</v>
       </c>
     </row>
     <row r="4">
@@ -496,7 +496,7 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>45497</v>
+        <v>45504</v>
       </c>
     </row>
     <row r="7">
@@ -506,7 +506,7 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>45504</v>
+        <v>45511</v>
       </c>
     </row>
     <row r="8">
@@ -516,7 +516,7 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>45503</v>
+        <v>45510</v>
       </c>
     </row>
     <row r="9">
@@ -526,7 +526,7 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>45510</v>
+        <v>45517</v>
       </c>
     </row>
     <row r="10">
@@ -536,7 +536,7 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>45502</v>
+        <v>45509</v>
       </c>
     </row>
     <row r="11">
@@ -546,7 +546,7 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>45509</v>
+        <v>45516</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added spot in cluster, shorter zip, reduced count of strikes in cluster
</commit_message>
<xml_diff>
--- a/symbols.xlsx
+++ b/symbols.xlsx
@@ -536,7 +536,7 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>45509</v>
+        <v>45516</v>
       </c>
     </row>
     <row r="11">
@@ -546,7 +546,7 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>45516</v>
+        <v>45523</v>
       </c>
     </row>
   </sheetData>

</xml_diff>